<commit_message>
add sick leave 16 april 2025
</commit_message>
<xml_diff>
--- a/16_Period_20_Mar_2025_sd_19_Apr_2025/Timesheet Danamon_Bayu Bagus Bagaswara_April.xlsx
+++ b/16_Period_20_Mar_2025_sd_19_Apr_2025/Timesheet Danamon_Bayu Bagus Bagaswara_April.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\16_Period_20_Mar_2025_sd_19_Apr_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CFC6BC-6A9C-4414-AC20-2CE49E26BC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2064FBD1-8E1C-4F09-A231-83933B5A2BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{287076C2-500C-4AE4-B01E-3C74A6B599A0}"/>
   </bookViews>
@@ -1561,7 +1561,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1964,9 +1964,42 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2069,30 +2102,6 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2145,18 +2154,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2796,12 +2793,12 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="142" t="s">
+      <c r="N5" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="153"/>
+      <c r="Q5" s="153"/>
     </row>
     <row r="6" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
@@ -2826,12 +2823,12 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="141" t="s">
+      <c r="N6" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:35" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2854,13 +2851,13 @@
       <c r="Q7" s="76"/>
     </row>
     <row r="9" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="175" t="s">
+      <c r="C9" s="143" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
@@ -2983,7 +2980,7 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="AH9" s="139" t="s">
+      <c r="AH9" s="144" t="s">
         <v>23</v>
       </c>
       <c r="AI9" s="90" t="s">
@@ -2991,9 +2988,9 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="175"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="175"/>
+      <c r="A10" s="143"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AG10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45536</v>
@@ -3085,7 +3082,7 @@
       <c r="AG10" s="51">
         <v>45565</v>
       </c>
-      <c r="AH10" s="139"/>
+      <c r="AH10" s="144"/>
       <c r="AI10" s="90"/>
     </row>
     <row r="11" spans="1:35" ht="17" x14ac:dyDescent="0.4">
@@ -3697,11 +3694,11 @@
       <c r="AI21" s="73"/>
     </row>
     <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="177"/>
-      <c r="C22" s="178"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57">
         <v>8</v>
@@ -3745,11 +3742,11 @@
       <c r="AI22" s="73"/>
     </row>
     <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="178"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="57"/>
       <c r="E23" s="57"/>
       <c r="F23" s="57">
@@ -3789,11 +3786,11 @@
       <c r="AI23" s="73"/>
     </row>
     <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="179" t="s">
+      <c r="A24" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="180"/>
-      <c r="C24" s="181"/>
+      <c r="B24" s="149"/>
+      <c r="C24" s="150"/>
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
       <c r="F24" s="57"/>
@@ -3833,11 +3830,11 @@
       <c r="AI24" s="73"/>
     </row>
     <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="176" t="s">
+      <c r="A25" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="177"/>
-      <c r="C25" s="178"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="147"/>
       <c r="D25" s="57"/>
       <c r="E25" s="57">
         <f t="shared" ref="E25:AB25" si="1">SUM(E11:E20)</f>
@@ -3968,145 +3965,145 @@
         <v>42</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="143"/>
-      <c r="S27" s="162" t="s">
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
+      <c r="H27" s="154"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="154"/>
+      <c r="S27" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="163"/>
-      <c r="U27" s="163"/>
-      <c r="V27" s="163"/>
-      <c r="W27" s="163"/>
-      <c r="X27" s="163"/>
-      <c r="Y27" s="163"/>
-      <c r="Z27" s="163"/>
-      <c r="AA27" s="164"/>
-      <c r="AC27" s="170" t="s">
+      <c r="T27" s="174"/>
+      <c r="U27" s="174"/>
+      <c r="V27" s="174"/>
+      <c r="W27" s="174"/>
+      <c r="X27" s="174"/>
+      <c r="Y27" s="174"/>
+      <c r="Z27" s="174"/>
+      <c r="AA27" s="175"/>
+      <c r="AC27" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="AD27" s="171"/>
-      <c r="AE27" s="171"/>
-      <c r="AF27" s="171"/>
-      <c r="AG27" s="171"/>
-      <c r="AH27" s="171"/>
-      <c r="AI27" s="171"/>
-      <c r="AJ27" s="172"/>
+      <c r="AD27" s="182"/>
+      <c r="AE27" s="182"/>
+      <c r="AF27" s="182"/>
+      <c r="AG27" s="182"/>
+      <c r="AH27" s="182"/>
+      <c r="AI27" s="182"/>
+      <c r="AJ27" s="183"/>
     </row>
     <row r="28" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="69"/>
       <c r="B28" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="143"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="143"/>
-      <c r="I28" s="143"/>
-      <c r="J28" s="143"/>
-      <c r="S28" s="153" t="s">
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
+      <c r="H28" s="154"/>
+      <c r="I28" s="154"/>
+      <c r="J28" s="154"/>
+      <c r="S28" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="T28" s="154"/>
-      <c r="U28" s="144" t="s">
+      <c r="T28" s="165"/>
+      <c r="U28" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="145"/>
-      <c r="W28" s="145"/>
-      <c r="X28" s="145"/>
-      <c r="Y28" s="145"/>
-      <c r="Z28" s="145"/>
-      <c r="AA28" s="146"/>
-      <c r="AC28" s="159" t="s">
+      <c r="V28" s="156"/>
+      <c r="W28" s="156"/>
+      <c r="X28" s="156"/>
+      <c r="Y28" s="156"/>
+      <c r="Z28" s="156"/>
+      <c r="AA28" s="157"/>
+      <c r="AC28" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="AD28" s="145"/>
-      <c r="AE28" s="145"/>
-      <c r="AF28" s="145"/>
-      <c r="AG28" s="145"/>
-      <c r="AH28" s="145"/>
-      <c r="AI28" s="145"/>
-      <c r="AJ28" s="146"/>
+      <c r="AD28" s="156"/>
+      <c r="AE28" s="156"/>
+      <c r="AF28" s="156"/>
+      <c r="AG28" s="156"/>
+      <c r="AH28" s="156"/>
+      <c r="AI28" s="156"/>
+      <c r="AJ28" s="157"/>
     </row>
     <row r="29" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="70"/>
       <c r="B29" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="143"/>
-      <c r="S29" s="155"/>
-      <c r="T29" s="156"/>
-      <c r="U29" s="147"/>
-      <c r="V29" s="148"/>
-      <c r="W29" s="148"/>
-      <c r="X29" s="148"/>
-      <c r="Y29" s="148"/>
-      <c r="Z29" s="148"/>
-      <c r="AA29" s="149"/>
-      <c r="AC29" s="160"/>
-      <c r="AD29" s="148"/>
-      <c r="AE29" s="148"/>
-      <c r="AF29" s="148"/>
-      <c r="AG29" s="148"/>
-      <c r="AH29" s="148"/>
-      <c r="AI29" s="148"/>
-      <c r="AJ29" s="149"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
+      <c r="H29" s="154"/>
+      <c r="I29" s="154"/>
+      <c r="J29" s="154"/>
+      <c r="S29" s="166"/>
+      <c r="T29" s="167"/>
+      <c r="U29" s="158"/>
+      <c r="V29" s="159"/>
+      <c r="W29" s="159"/>
+      <c r="X29" s="159"/>
+      <c r="Y29" s="159"/>
+      <c r="Z29" s="159"/>
+      <c r="AA29" s="160"/>
+      <c r="AC29" s="171"/>
+      <c r="AD29" s="159"/>
+      <c r="AE29" s="159"/>
+      <c r="AF29" s="159"/>
+      <c r="AG29" s="159"/>
+      <c r="AH29" s="159"/>
+      <c r="AI29" s="159"/>
+      <c r="AJ29" s="160"/>
     </row>
     <row r="30" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="71"/>
       <c r="B30" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="S30" s="155"/>
-      <c r="T30" s="156"/>
-      <c r="U30" s="147"/>
-      <c r="V30" s="148"/>
-      <c r="W30" s="148"/>
-      <c r="X30" s="148"/>
-      <c r="Y30" s="148"/>
-      <c r="Z30" s="148"/>
-      <c r="AA30" s="149"/>
-      <c r="AC30" s="160"/>
-      <c r="AD30" s="148"/>
-      <c r="AE30" s="148"/>
-      <c r="AF30" s="148"/>
-      <c r="AG30" s="148"/>
-      <c r="AH30" s="148"/>
-      <c r="AI30" s="148"/>
-      <c r="AJ30" s="149"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="154"/>
+      <c r="S30" s="166"/>
+      <c r="T30" s="167"/>
+      <c r="U30" s="158"/>
+      <c r="V30" s="159"/>
+      <c r="W30" s="159"/>
+      <c r="X30" s="159"/>
+      <c r="Y30" s="159"/>
+      <c r="Z30" s="159"/>
+      <c r="AA30" s="160"/>
+      <c r="AC30" s="171"/>
+      <c r="AD30" s="159"/>
+      <c r="AE30" s="159"/>
+      <c r="AF30" s="159"/>
+      <c r="AG30" s="159"/>
+      <c r="AH30" s="159"/>
+      <c r="AI30" s="159"/>
+      <c r="AJ30" s="160"/>
     </row>
     <row r="31" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S31" s="155"/>
-      <c r="T31" s="156"/>
-      <c r="U31" s="147"/>
-      <c r="V31" s="148"/>
-      <c r="W31" s="148"/>
-      <c r="X31" s="148"/>
-      <c r="Y31" s="148"/>
-      <c r="Z31" s="148"/>
-      <c r="AA31" s="149"/>
-      <c r="AC31" s="160"/>
-      <c r="AD31" s="148"/>
-      <c r="AE31" s="148"/>
-      <c r="AF31" s="148"/>
-      <c r="AG31" s="148"/>
-      <c r="AH31" s="148"/>
-      <c r="AI31" s="148"/>
-      <c r="AJ31" s="149"/>
+      <c r="S31" s="166"/>
+      <c r="T31" s="167"/>
+      <c r="U31" s="158"/>
+      <c r="V31" s="159"/>
+      <c r="W31" s="159"/>
+      <c r="X31" s="159"/>
+      <c r="Y31" s="159"/>
+      <c r="Z31" s="159"/>
+      <c r="AA31" s="160"/>
+      <c r="AC31" s="171"/>
+      <c r="AD31" s="159"/>
+      <c r="AE31" s="159"/>
+      <c r="AF31" s="159"/>
+      <c r="AG31" s="159"/>
+      <c r="AH31" s="159"/>
+      <c r="AI31" s="159"/>
+      <c r="AJ31" s="160"/>
     </row>
     <row r="32" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
@@ -4119,29 +4116,29 @@
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
-      <c r="S32" s="165"/>
-      <c r="T32" s="166"/>
-      <c r="U32" s="167"/>
-      <c r="V32" s="168"/>
-      <c r="W32" s="168"/>
-      <c r="X32" s="168"/>
-      <c r="Y32" s="168"/>
-      <c r="Z32" s="168"/>
-      <c r="AA32" s="169"/>
-      <c r="AC32" s="173"/>
-      <c r="AD32" s="168"/>
-      <c r="AE32" s="168"/>
-      <c r="AF32" s="168"/>
-      <c r="AG32" s="168"/>
-      <c r="AH32" s="168"/>
-      <c r="AI32" s="168"/>
-      <c r="AJ32" s="169"/>
+      <c r="S32" s="176"/>
+      <c r="T32" s="177"/>
+      <c r="U32" s="178"/>
+      <c r="V32" s="179"/>
+      <c r="W32" s="179"/>
+      <c r="X32" s="179"/>
+      <c r="Y32" s="179"/>
+      <c r="Z32" s="179"/>
+      <c r="AA32" s="180"/>
+      <c r="AC32" s="184"/>
+      <c r="AD32" s="179"/>
+      <c r="AE32" s="179"/>
+      <c r="AF32" s="179"/>
+      <c r="AG32" s="179"/>
+      <c r="AH32" s="179"/>
+      <c r="AI32" s="179"/>
+      <c r="AJ32" s="180"/>
     </row>
     <row r="33" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="140" t="s">
+      <c r="A33" s="151" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="140"/>
+      <c r="B33" s="151"/>
       <c r="C33" s="63">
         <f>COUNTIF(D24:AG24,"=8")</f>
         <v>1</v>
@@ -4151,29 +4148,29 @@
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
-      <c r="S33" s="153" t="s">
+      <c r="S33" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="T33" s="154"/>
-      <c r="U33" s="144" t="s">
+      <c r="T33" s="165"/>
+      <c r="U33" s="155" t="s">
         <v>54</v>
       </c>
-      <c r="V33" s="145"/>
-      <c r="W33" s="145"/>
-      <c r="X33" s="145"/>
-      <c r="Y33" s="145"/>
-      <c r="Z33" s="145"/>
-      <c r="AA33" s="146"/>
-      <c r="AC33" s="159" t="s">
+      <c r="V33" s="156"/>
+      <c r="W33" s="156"/>
+      <c r="X33" s="156"/>
+      <c r="Y33" s="156"/>
+      <c r="Z33" s="156"/>
+      <c r="AA33" s="157"/>
+      <c r="AC33" s="170" t="s">
         <v>55</v>
       </c>
-      <c r="AD33" s="145"/>
-      <c r="AE33" s="145"/>
-      <c r="AF33" s="145"/>
-      <c r="AG33" s="145"/>
-      <c r="AH33" s="145"/>
-      <c r="AI33" s="145"/>
-      <c r="AJ33" s="146"/>
+      <c r="AD33" s="156"/>
+      <c r="AE33" s="156"/>
+      <c r="AF33" s="156"/>
+      <c r="AG33" s="156"/>
+      <c r="AH33" s="156"/>
+      <c r="AI33" s="156"/>
+      <c r="AJ33" s="157"/>
     </row>
     <row r="34" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="63" t="s">
@@ -4189,23 +4186,23 @@
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
-      <c r="S34" s="155"/>
-      <c r="T34" s="156"/>
-      <c r="U34" s="147"/>
-      <c r="V34" s="148"/>
-      <c r="W34" s="148"/>
-      <c r="X34" s="148"/>
-      <c r="Y34" s="148"/>
-      <c r="Z34" s="148"/>
-      <c r="AA34" s="149"/>
-      <c r="AC34" s="160"/>
-      <c r="AD34" s="148"/>
-      <c r="AE34" s="148"/>
-      <c r="AF34" s="148"/>
-      <c r="AG34" s="148"/>
-      <c r="AH34" s="148"/>
-      <c r="AI34" s="148"/>
-      <c r="AJ34" s="149"/>
+      <c r="S34" s="166"/>
+      <c r="T34" s="167"/>
+      <c r="U34" s="158"/>
+      <c r="V34" s="159"/>
+      <c r="W34" s="159"/>
+      <c r="X34" s="159"/>
+      <c r="Y34" s="159"/>
+      <c r="Z34" s="159"/>
+      <c r="AA34" s="160"/>
+      <c r="AC34" s="171"/>
+      <c r="AD34" s="159"/>
+      <c r="AE34" s="159"/>
+      <c r="AF34" s="159"/>
+      <c r="AG34" s="159"/>
+      <c r="AH34" s="159"/>
+      <c r="AI34" s="159"/>
+      <c r="AJ34" s="160"/>
     </row>
     <row r="35" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="63" t="s">
@@ -4221,23 +4218,23 @@
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
-      <c r="S35" s="155"/>
-      <c r="T35" s="156"/>
-      <c r="U35" s="147"/>
-      <c r="V35" s="148"/>
-      <c r="W35" s="148"/>
-      <c r="X35" s="148"/>
-      <c r="Y35" s="148"/>
-      <c r="Z35" s="148"/>
-      <c r="AA35" s="149"/>
-      <c r="AC35" s="160"/>
-      <c r="AD35" s="148"/>
-      <c r="AE35" s="148"/>
-      <c r="AF35" s="148"/>
-      <c r="AG35" s="148"/>
-      <c r="AH35" s="148"/>
-      <c r="AI35" s="148"/>
-      <c r="AJ35" s="149"/>
+      <c r="S35" s="166"/>
+      <c r="T35" s="167"/>
+      <c r="U35" s="158"/>
+      <c r="V35" s="159"/>
+      <c r="W35" s="159"/>
+      <c r="X35" s="159"/>
+      <c r="Y35" s="159"/>
+      <c r="Z35" s="159"/>
+      <c r="AA35" s="160"/>
+      <c r="AC35" s="171"/>
+      <c r="AD35" s="159"/>
+      <c r="AE35" s="159"/>
+      <c r="AF35" s="159"/>
+      <c r="AG35" s="159"/>
+      <c r="AH35" s="159"/>
+      <c r="AI35" s="159"/>
+      <c r="AJ35" s="160"/>
     </row>
     <row r="36" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="63" t="s">
@@ -4253,29 +4250,29 @@
       <c r="F36" s="44"/>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
-      <c r="S36" s="155"/>
-      <c r="T36" s="156"/>
-      <c r="U36" s="147"/>
-      <c r="V36" s="148"/>
-      <c r="W36" s="148"/>
-      <c r="X36" s="148"/>
-      <c r="Y36" s="148"/>
-      <c r="Z36" s="148"/>
-      <c r="AA36" s="149"/>
-      <c r="AC36" s="160"/>
-      <c r="AD36" s="148"/>
-      <c r="AE36" s="148"/>
-      <c r="AF36" s="148"/>
-      <c r="AG36" s="148"/>
-      <c r="AH36" s="148"/>
-      <c r="AI36" s="148"/>
-      <c r="AJ36" s="149"/>
+      <c r="S36" s="166"/>
+      <c r="T36" s="167"/>
+      <c r="U36" s="158"/>
+      <c r="V36" s="159"/>
+      <c r="W36" s="159"/>
+      <c r="X36" s="159"/>
+      <c r="Y36" s="159"/>
+      <c r="Z36" s="159"/>
+      <c r="AA36" s="160"/>
+      <c r="AC36" s="171"/>
+      <c r="AD36" s="159"/>
+      <c r="AE36" s="159"/>
+      <c r="AF36" s="159"/>
+      <c r="AG36" s="159"/>
+      <c r="AH36" s="159"/>
+      <c r="AI36" s="159"/>
+      <c r="AJ36" s="160"/>
     </row>
     <row r="37" spans="1:36" ht="38.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="174" t="s">
+      <c r="A37" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="174"/>
+      <c r="B37" s="142"/>
       <c r="C37" s="63">
         <f>COUNTIF(D25:AG25,"&gt;0")</f>
         <v>20</v>
@@ -4285,23 +4282,23 @@
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
       <c r="H37" s="44"/>
-      <c r="S37" s="157"/>
-      <c r="T37" s="158"/>
-      <c r="U37" s="150"/>
-      <c r="V37" s="151"/>
-      <c r="W37" s="151"/>
-      <c r="X37" s="151"/>
-      <c r="Y37" s="151"/>
-      <c r="Z37" s="151"/>
-      <c r="AA37" s="152"/>
-      <c r="AC37" s="161"/>
-      <c r="AD37" s="151"/>
-      <c r="AE37" s="151"/>
-      <c r="AF37" s="151"/>
-      <c r="AG37" s="151"/>
-      <c r="AH37" s="151"/>
-      <c r="AI37" s="151"/>
-      <c r="AJ37" s="152"/>
+      <c r="S37" s="168"/>
+      <c r="T37" s="169"/>
+      <c r="U37" s="161"/>
+      <c r="V37" s="162"/>
+      <c r="W37" s="162"/>
+      <c r="X37" s="162"/>
+      <c r="Y37" s="162"/>
+      <c r="Z37" s="162"/>
+      <c r="AA37" s="163"/>
+      <c r="AC37" s="172"/>
+      <c r="AD37" s="162"/>
+      <c r="AE37" s="162"/>
+      <c r="AF37" s="162"/>
+      <c r="AG37" s="162"/>
+      <c r="AH37" s="162"/>
+      <c r="AI37" s="162"/>
+      <c r="AJ37" s="163"/>
     </row>
     <row r="38" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="63" t="s">
@@ -4341,10 +4338,10 @@
       <c r="H40" s="44"/>
     </row>
     <row r="41" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="142" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="174"/>
+      <c r="B41" s="142"/>
       <c r="C41" s="63">
         <f>AH25</f>
         <v>160</v>
@@ -4356,10 +4353,10 @@
       <c r="H41" s="44"/>
     </row>
     <row r="42" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="174" t="s">
+      <c r="A42" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="174"/>
+      <c r="B42" s="142"/>
       <c r="C42" s="63">
         <v>45</v>
       </c>
@@ -4488,15 +4485,6 @@
     <row r="53" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="C9:C10"/>
     <mergeCell ref="AH9:AH10"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="N6:Q6"/>
@@ -4511,6 +4499,15 @@
     <mergeCell ref="AC27:AJ27"/>
     <mergeCell ref="AC28:AJ32"/>
     <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="expression" dxfId="11" priority="26">
@@ -4555,8 +4552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA136F23-B726-450C-8838-7114D5303DC9}">
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4684,12 +4681,12 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="142" t="s">
+      <c r="N5" s="153" t="s">
         <v>167</v>
       </c>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="153"/>
+      <c r="Q5" s="153"/>
     </row>
     <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
@@ -4714,12 +4711,12 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="141" t="s">
+      <c r="N6" s="152" t="s">
         <v>168</v>
       </c>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
+      <c r="O6" s="152"/>
+      <c r="P6" s="152"/>
+      <c r="Q6" s="152"/>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:36" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -4742,13 +4739,13 @@
       <c r="Q7" s="76"/>
     </row>
     <row r="9" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="175" t="s">
+      <c r="C9" s="143" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
@@ -4875,7 +4872,7 @@
         <f t="shared" si="0"/>
         <v>Sat</v>
       </c>
-      <c r="AI9" s="139" t="s">
+      <c r="AI9" s="144" t="s">
         <v>23</v>
       </c>
       <c r="AJ9" s="90" t="s">
@@ -4883,9 +4880,9 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="175"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="175"/>
+      <c r="A10" s="143"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AH10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45736</v>
@@ -4980,7 +4977,7 @@
       <c r="AH10" s="51">
         <v>45766</v>
       </c>
-      <c r="AI10" s="139"/>
+      <c r="AI10" s="144"/>
       <c r="AJ10" s="90"/>
     </row>
     <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.4">
@@ -5025,7 +5022,7 @@
     </row>
     <row r="12" spans="1:36" ht="153" x14ac:dyDescent="0.4">
       <c r="A12" s="88"/>
-      <c r="B12" s="203" t="s">
+      <c r="B12" s="141" t="s">
         <v>174</v>
       </c>
       <c r="C12" s="57"/>
@@ -5037,20 +5034,20 @@
       <c r="I12" s="50"/>
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
-      <c r="L12" s="202"/>
+      <c r="L12" s="50"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
-      <c r="O12" s="202"/>
-      <c r="P12" s="202"/>
-      <c r="Q12" s="202"/>
-      <c r="R12" s="202"/>
-      <c r="S12" s="202"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
       <c r="T12" s="50"/>
       <c r="U12" s="50"/>
-      <c r="V12" s="202"/>
-      <c r="W12" s="201"/>
-      <c r="X12" s="201"/>
-      <c r="Y12" s="201"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="140"/>
+      <c r="X12" s="140"/>
+      <c r="Y12" s="140"/>
       <c r="Z12" s="50"/>
       <c r="AA12" s="50"/>
       <c r="AB12" s="50"/>
@@ -5078,20 +5075,20 @@
       <c r="I13" s="50"/>
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
-      <c r="L13" s="202"/>
+      <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
-      <c r="O13" s="202"/>
-      <c r="P13" s="202"/>
-      <c r="Q13" s="202"/>
-      <c r="R13" s="202"/>
-      <c r="S13" s="202"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
       <c r="T13" s="50"/>
       <c r="U13" s="50"/>
-      <c r="V13" s="202"/>
-      <c r="W13" s="201"/>
-      <c r="X13" s="201"/>
-      <c r="Y13" s="201"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="140"/>
+      <c r="X13" s="140"/>
+      <c r="Y13" s="140"/>
       <c r="Z13" s="50"/>
       <c r="AA13" s="50"/>
       <c r="AB13" s="50"/>
@@ -5119,20 +5116,20 @@
       <c r="I14" s="50"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
-      <c r="L14" s="202"/>
+      <c r="L14" s="50"/>
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
-      <c r="O14" s="202"/>
-      <c r="P14" s="202"/>
-      <c r="Q14" s="202"/>
-      <c r="R14" s="202"/>
-      <c r="S14" s="202"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
       <c r="T14" s="50"/>
       <c r="U14" s="50"/>
-      <c r="V14" s="202"/>
-      <c r="W14" s="201"/>
-      <c r="X14" s="201"/>
-      <c r="Y14" s="201"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="140"/>
+      <c r="X14" s="140"/>
+      <c r="Y14" s="140"/>
       <c r="Z14" s="50"/>
       <c r="AA14" s="50"/>
       <c r="AB14" s="50"/>
@@ -5160,20 +5157,20 @@
       <c r="I15" s="50"/>
       <c r="J15" s="50"/>
       <c r="K15" s="50"/>
-      <c r="L15" s="202"/>
+      <c r="L15" s="50"/>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
-      <c r="O15" s="202"/>
-      <c r="P15" s="202"/>
-      <c r="Q15" s="202"/>
-      <c r="R15" s="202"/>
-      <c r="S15" s="202"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
       <c r="T15" s="50"/>
       <c r="U15" s="50"/>
-      <c r="V15" s="202"/>
-      <c r="W15" s="201"/>
-      <c r="X15" s="201"/>
-      <c r="Y15" s="201"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="140"/>
+      <c r="X15" s="140"/>
+      <c r="Y15" s="140"/>
       <c r="Z15" s="50"/>
       <c r="AA15" s="50"/>
       <c r="AB15" s="50"/>
@@ -5201,20 +5198,20 @@
       <c r="I16" s="50"/>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
-      <c r="L16" s="202"/>
+      <c r="L16" s="50"/>
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
-      <c r="O16" s="202"/>
-      <c r="P16" s="202"/>
-      <c r="Q16" s="202"/>
-      <c r="R16" s="202"/>
-      <c r="S16" s="202"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
       <c r="T16" s="50"/>
       <c r="U16" s="50"/>
-      <c r="V16" s="202"/>
-      <c r="W16" s="201"/>
-      <c r="X16" s="201"/>
-      <c r="Y16" s="201"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="140"/>
+      <c r="X16" s="140"/>
+      <c r="Y16" s="140"/>
       <c r="Z16" s="50"/>
       <c r="AA16" s="50"/>
       <c r="AB16" s="50"/>
@@ -5242,20 +5239,20 @@
       <c r="I17" s="50"/>
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
-      <c r="L17" s="202"/>
+      <c r="L17" s="50"/>
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
-      <c r="O17" s="202"/>
-      <c r="P17" s="202"/>
-      <c r="Q17" s="202"/>
-      <c r="R17" s="202"/>
-      <c r="S17" s="202"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
       <c r="T17" s="50"/>
       <c r="U17" s="50"/>
-      <c r="V17" s="202"/>
-      <c r="W17" s="201"/>
-      <c r="X17" s="201"/>
-      <c r="Y17" s="201"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="140"/>
+      <c r="X17" s="140"/>
+      <c r="Y17" s="140"/>
       <c r="Z17" s="50"/>
       <c r="AA17" s="50"/>
       <c r="AB17" s="50"/>
@@ -5283,20 +5280,20 @@
       <c r="I18" s="50"/>
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
-      <c r="L18" s="202"/>
+      <c r="L18" s="50"/>
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
-      <c r="O18" s="202"/>
-      <c r="P18" s="202"/>
-      <c r="Q18" s="202"/>
-      <c r="R18" s="202"/>
-      <c r="S18" s="202"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
       <c r="T18" s="50"/>
       <c r="U18" s="50"/>
-      <c r="V18" s="202"/>
-      <c r="W18" s="201"/>
-      <c r="X18" s="201"/>
-      <c r="Y18" s="201"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="140"/>
+      <c r="X18" s="140"/>
+      <c r="Y18" s="140"/>
       <c r="Z18" s="50"/>
       <c r="AA18" s="50"/>
       <c r="AB18" s="50"/>
@@ -5324,20 +5321,20 @@
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
-      <c r="L19" s="202"/>
+      <c r="L19" s="50"/>
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
-      <c r="O19" s="202"/>
-      <c r="P19" s="202"/>
-      <c r="Q19" s="202"/>
-      <c r="R19" s="202"/>
-      <c r="S19" s="202"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
       <c r="T19" s="50"/>
       <c r="U19" s="50"/>
-      <c r="V19" s="202"/>
-      <c r="W19" s="201"/>
-      <c r="X19" s="201"/>
-      <c r="Y19" s="201"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="140"/>
+      <c r="X19" s="140"/>
+      <c r="Y19" s="140"/>
       <c r="Z19" s="50"/>
       <c r="AA19" s="50"/>
       <c r="AB19" s="50"/>
@@ -5365,20 +5362,20 @@
       <c r="I20" s="50"/>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
-      <c r="L20" s="202"/>
+      <c r="L20" s="50"/>
       <c r="M20" s="50"/>
       <c r="N20" s="50"/>
-      <c r="O20" s="202"/>
-      <c r="P20" s="202"/>
-      <c r="Q20" s="202"/>
-      <c r="R20" s="202"/>
-      <c r="S20" s="202"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
       <c r="T20" s="50"/>
       <c r="U20" s="50"/>
-      <c r="V20" s="202"/>
-      <c r="W20" s="201"/>
-      <c r="X20" s="201"/>
-      <c r="Y20" s="201"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="140"/>
+      <c r="X20" s="140"/>
+      <c r="Y20" s="140"/>
       <c r="Z20" s="50"/>
       <c r="AA20" s="50"/>
       <c r="AB20" s="50"/>
@@ -5406,20 +5403,20 @@
       <c r="I21" s="50"/>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
-      <c r="L21" s="202"/>
+      <c r="L21" s="50"/>
       <c r="M21" s="50"/>
       <c r="N21" s="50"/>
-      <c r="O21" s="202"/>
-      <c r="P21" s="202"/>
-      <c r="Q21" s="202"/>
-      <c r="R21" s="202"/>
-      <c r="S21" s="202"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
       <c r="T21" s="50"/>
       <c r="U21" s="50"/>
-      <c r="V21" s="202"/>
-      <c r="W21" s="201"/>
-      <c r="X21" s="201"/>
-      <c r="Y21" s="201"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="140"/>
+      <c r="X21" s="140"/>
+      <c r="Y21" s="140"/>
       <c r="Z21" s="50"/>
       <c r="AA21" s="50"/>
       <c r="AB21" s="50"/>
@@ -5447,20 +5444,20 @@
       <c r="I22" s="50"/>
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
-      <c r="L22" s="202"/>
+      <c r="L22" s="50"/>
       <c r="M22" s="50"/>
       <c r="N22" s="50"/>
-      <c r="O22" s="202"/>
-      <c r="P22" s="202"/>
-      <c r="Q22" s="202"/>
-      <c r="R22" s="202"/>
-      <c r="S22" s="202"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="50"/>
       <c r="T22" s="50"/>
       <c r="U22" s="50"/>
-      <c r="V22" s="202"/>
-      <c r="W22" s="201"/>
-      <c r="X22" s="201"/>
-      <c r="Y22" s="201"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="140"/>
+      <c r="X22" s="140"/>
+      <c r="Y22" s="140"/>
       <c r="Z22" s="50"/>
       <c r="AA22" s="50"/>
       <c r="AB22" s="50"/>
@@ -5488,20 +5485,20 @@
       <c r="I23" s="50"/>
       <c r="J23" s="50"/>
       <c r="K23" s="50"/>
-      <c r="L23" s="202"/>
+      <c r="L23" s="50"/>
       <c r="M23" s="50"/>
       <c r="N23" s="50"/>
-      <c r="O23" s="202"/>
-      <c r="P23" s="202"/>
-      <c r="Q23" s="202"/>
-      <c r="R23" s="202"/>
-      <c r="S23" s="202"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
       <c r="T23" s="50"/>
       <c r="U23" s="50"/>
-      <c r="V23" s="202"/>
-      <c r="W23" s="201"/>
-      <c r="X23" s="201"/>
-      <c r="Y23" s="201"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="140"/>
+      <c r="X23" s="140"/>
+      <c r="Y23" s="140"/>
       <c r="Z23" s="50"/>
       <c r="AA23" s="50"/>
       <c r="AB23" s="50"/>
@@ -5529,20 +5526,20 @@
       <c r="I24" s="50"/>
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
-      <c r="L24" s="202"/>
+      <c r="L24" s="50"/>
       <c r="M24" s="50"/>
       <c r="N24" s="50"/>
-      <c r="O24" s="202"/>
-      <c r="P24" s="202"/>
-      <c r="Q24" s="202"/>
-      <c r="R24" s="202"/>
-      <c r="S24" s="202"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
       <c r="T24" s="50"/>
       <c r="U24" s="50"/>
-      <c r="V24" s="202"/>
-      <c r="W24" s="201"/>
-      <c r="X24" s="201"/>
-      <c r="Y24" s="201"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="140"/>
+      <c r="X24" s="140"/>
+      <c r="Y24" s="140"/>
       <c r="Z24" s="50"/>
       <c r="AA24" s="50"/>
       <c r="AB24" s="50"/>
@@ -5570,20 +5567,20 @@
       <c r="I25" s="50"/>
       <c r="J25" s="50"/>
       <c r="K25" s="50"/>
-      <c r="L25" s="202"/>
+      <c r="L25" s="50"/>
       <c r="M25" s="50"/>
       <c r="N25" s="50"/>
-      <c r="O25" s="202"/>
-      <c r="P25" s="202"/>
-      <c r="Q25" s="202"/>
-      <c r="R25" s="202"/>
-      <c r="S25" s="202"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
       <c r="T25" s="50"/>
       <c r="U25" s="50"/>
-      <c r="V25" s="202"/>
-      <c r="W25" s="201"/>
-      <c r="X25" s="201"/>
-      <c r="Y25" s="201"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="140"/>
+      <c r="X25" s="140"/>
+      <c r="Y25" s="140"/>
       <c r="Z25" s="50"/>
       <c r="AA25" s="50"/>
       <c r="AB25" s="50"/>
@@ -5611,20 +5608,20 @@
       <c r="I26" s="50"/>
       <c r="J26" s="50"/>
       <c r="K26" s="50"/>
-      <c r="L26" s="202"/>
+      <c r="L26" s="50"/>
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
-      <c r="O26" s="202"/>
-      <c r="P26" s="202"/>
-      <c r="Q26" s="202"/>
-      <c r="R26" s="202"/>
-      <c r="S26" s="202"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
       <c r="T26" s="50"/>
       <c r="U26" s="50"/>
-      <c r="V26" s="202"/>
-      <c r="W26" s="201"/>
-      <c r="X26" s="201"/>
-      <c r="Y26" s="201"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="140"/>
+      <c r="X26" s="140"/>
+      <c r="Y26" s="140"/>
       <c r="Z26" s="50"/>
       <c r="AA26" s="50"/>
       <c r="AB26" s="50"/>
@@ -5652,20 +5649,20 @@
       <c r="I27" s="50"/>
       <c r="J27" s="50"/>
       <c r="K27" s="50"/>
-      <c r="L27" s="202"/>
+      <c r="L27" s="50"/>
       <c r="M27" s="50"/>
       <c r="N27" s="50"/>
-      <c r="O27" s="202"/>
-      <c r="P27" s="202"/>
-      <c r="Q27" s="202"/>
-      <c r="R27" s="202"/>
-      <c r="S27" s="202"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
       <c r="T27" s="50"/>
       <c r="U27" s="50"/>
-      <c r="V27" s="202"/>
-      <c r="W27" s="201"/>
-      <c r="X27" s="201"/>
-      <c r="Y27" s="201"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="140"/>
+      <c r="X27" s="140"/>
+      <c r="Y27" s="140"/>
       <c r="Z27" s="50"/>
       <c r="AA27" s="50"/>
       <c r="AB27" s="50"/>
@@ -5693,20 +5690,20 @@
       <c r="I28" s="50"/>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
-      <c r="L28" s="202"/>
+      <c r="L28" s="50"/>
       <c r="M28" s="50"/>
       <c r="N28" s="50"/>
-      <c r="O28" s="202"/>
-      <c r="P28" s="202"/>
-      <c r="Q28" s="202"/>
-      <c r="R28" s="202"/>
-      <c r="S28" s="202"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
       <c r="T28" s="50"/>
       <c r="U28" s="50"/>
-      <c r="V28" s="202"/>
-      <c r="W28" s="201"/>
-      <c r="X28" s="201"/>
-      <c r="Y28" s="201"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="140"/>
+      <c r="X28" s="140"/>
+      <c r="Y28" s="140"/>
       <c r="Z28" s="50"/>
       <c r="AA28" s="50"/>
       <c r="AB28" s="50"/>
@@ -5734,20 +5731,20 @@
       <c r="I29" s="50"/>
       <c r="J29" s="50"/>
       <c r="K29" s="50"/>
-      <c r="L29" s="202"/>
+      <c r="L29" s="50"/>
       <c r="M29" s="50"/>
       <c r="N29" s="50"/>
-      <c r="O29" s="202"/>
-      <c r="P29" s="202"/>
-      <c r="Q29" s="202"/>
-      <c r="R29" s="202"/>
-      <c r="S29" s="202"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
       <c r="T29" s="50"/>
       <c r="U29" s="50"/>
-      <c r="V29" s="202"/>
-      <c r="W29" s="201"/>
-      <c r="X29" s="201"/>
-      <c r="Y29" s="201"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="140"/>
+      <c r="X29" s="140"/>
+      <c r="Y29" s="140"/>
       <c r="Z29" s="50"/>
       <c r="AA29" s="50"/>
       <c r="AB29" s="50"/>
@@ -5775,20 +5772,20 @@
       <c r="I30" s="50"/>
       <c r="J30" s="50"/>
       <c r="K30" s="50"/>
-      <c r="L30" s="202"/>
+      <c r="L30" s="50"/>
       <c r="M30" s="50"/>
       <c r="N30" s="50"/>
-      <c r="O30" s="202"/>
-      <c r="P30" s="202"/>
-      <c r="Q30" s="202"/>
-      <c r="R30" s="202"/>
-      <c r="S30" s="202"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
       <c r="T30" s="50"/>
       <c r="U30" s="50"/>
-      <c r="V30" s="202"/>
-      <c r="W30" s="201"/>
-      <c r="X30" s="201"/>
-      <c r="Y30" s="201"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="140"/>
+      <c r="X30" s="140"/>
+      <c r="Y30" s="140"/>
       <c r="Z30" s="50"/>
       <c r="AA30" s="50"/>
       <c r="AB30" s="50"/>
@@ -5816,20 +5813,20 @@
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
-      <c r="L31" s="202"/>
+      <c r="L31" s="50"/>
       <c r="M31" s="50"/>
       <c r="N31" s="50"/>
-      <c r="O31" s="202"/>
-      <c r="P31" s="202"/>
-      <c r="Q31" s="202"/>
-      <c r="R31" s="202"/>
-      <c r="S31" s="202"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
       <c r="T31" s="50"/>
       <c r="U31" s="50"/>
-      <c r="V31" s="202"/>
-      <c r="W31" s="201"/>
-      <c r="X31" s="201"/>
-      <c r="Y31" s="201"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="140"/>
+      <c r="X31" s="140"/>
+      <c r="Y31" s="140"/>
       <c r="Z31" s="50"/>
       <c r="AA31" s="50"/>
       <c r="AB31" s="50"/>
@@ -5857,20 +5854,20 @@
       <c r="I32" s="50"/>
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
-      <c r="L32" s="202"/>
+      <c r="L32" s="50"/>
       <c r="M32" s="50"/>
       <c r="N32" s="50"/>
-      <c r="O32" s="202"/>
-      <c r="P32" s="202"/>
-      <c r="Q32" s="202"/>
-      <c r="R32" s="202"/>
-      <c r="S32" s="202"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
       <c r="T32" s="50"/>
       <c r="U32" s="50"/>
-      <c r="V32" s="202"/>
-      <c r="W32" s="201"/>
-      <c r="X32" s="201"/>
-      <c r="Y32" s="201"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="140"/>
+      <c r="X32" s="140"/>
+      <c r="Y32" s="140"/>
       <c r="Z32" s="50"/>
       <c r="AA32" s="50"/>
       <c r="AB32" s="50"/>
@@ -5898,20 +5895,20 @@
       <c r="I33" s="50"/>
       <c r="J33" s="50"/>
       <c r="K33" s="50"/>
-      <c r="L33" s="202"/>
+      <c r="L33" s="50"/>
       <c r="M33" s="50"/>
       <c r="N33" s="50"/>
-      <c r="O33" s="202"/>
-      <c r="P33" s="202"/>
-      <c r="Q33" s="202"/>
-      <c r="R33" s="202"/>
-      <c r="S33" s="202"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
       <c r="T33" s="50"/>
       <c r="U33" s="50"/>
-      <c r="V33" s="202"/>
-      <c r="W33" s="201"/>
-      <c r="X33" s="201"/>
-      <c r="Y33" s="201"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="140"/>
+      <c r="X33" s="140"/>
+      <c r="Y33" s="140"/>
       <c r="Z33" s="50"/>
       <c r="AA33" s="50"/>
       <c r="AB33" s="50"/>
@@ -5939,20 +5936,20 @@
       <c r="I34" s="50"/>
       <c r="J34" s="50"/>
       <c r="K34" s="50"/>
-      <c r="L34" s="202"/>
+      <c r="L34" s="50"/>
       <c r="M34" s="50"/>
       <c r="N34" s="50"/>
-      <c r="O34" s="202"/>
-      <c r="P34" s="202"/>
-      <c r="Q34" s="202"/>
-      <c r="R34" s="202"/>
-      <c r="S34" s="202"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
       <c r="T34" s="50"/>
       <c r="U34" s="50"/>
-      <c r="V34" s="202"/>
-      <c r="W34" s="201"/>
-      <c r="X34" s="201"/>
-      <c r="Y34" s="201"/>
+      <c r="V34" s="50"/>
+      <c r="W34" s="140"/>
+      <c r="X34" s="140"/>
+      <c r="Y34" s="140"/>
       <c r="Z34" s="50"/>
       <c r="AA34" s="50"/>
       <c r="AB34" s="50"/>
@@ -5980,20 +5977,20 @@
       <c r="I35" s="50"/>
       <c r="J35" s="50"/>
       <c r="K35" s="50"/>
-      <c r="L35" s="202"/>
+      <c r="L35" s="50"/>
       <c r="M35" s="50"/>
       <c r="N35" s="50"/>
-      <c r="O35" s="202"/>
-      <c r="P35" s="202"/>
-      <c r="Q35" s="202"/>
-      <c r="R35" s="202"/>
-      <c r="S35" s="202"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
       <c r="T35" s="50"/>
       <c r="U35" s="50"/>
-      <c r="V35" s="202"/>
-      <c r="W35" s="201"/>
-      <c r="X35" s="201"/>
-      <c r="Y35" s="201"/>
+      <c r="V35" s="50"/>
+      <c r="W35" s="140"/>
+      <c r="X35" s="140"/>
+      <c r="Y35" s="140"/>
       <c r="Z35" s="50"/>
       <c r="AA35" s="50"/>
       <c r="AB35" s="50"/>
@@ -6021,20 +6018,20 @@
       <c r="I36" s="50"/>
       <c r="J36" s="50"/>
       <c r="K36" s="50"/>
-      <c r="L36" s="202"/>
+      <c r="L36" s="50"/>
       <c r="M36" s="50"/>
       <c r="N36" s="50"/>
-      <c r="O36" s="202"/>
-      <c r="P36" s="202"/>
-      <c r="Q36" s="202"/>
-      <c r="R36" s="202"/>
-      <c r="S36" s="202"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
       <c r="T36" s="50"/>
       <c r="U36" s="50"/>
-      <c r="V36" s="202"/>
-      <c r="W36" s="201"/>
-      <c r="X36" s="201"/>
-      <c r="Y36" s="201"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="140"/>
+      <c r="X36" s="140"/>
+      <c r="Y36" s="140"/>
       <c r="Z36" s="50"/>
       <c r="AA36" s="50"/>
       <c r="AB36" s="50"/>
@@ -6062,20 +6059,20 @@
       <c r="I37" s="50"/>
       <c r="J37" s="50"/>
       <c r="K37" s="50"/>
-      <c r="L37" s="202"/>
+      <c r="L37" s="50"/>
       <c r="M37" s="50"/>
       <c r="N37" s="50"/>
-      <c r="O37" s="202"/>
-      <c r="P37" s="202"/>
-      <c r="Q37" s="202"/>
-      <c r="R37" s="202"/>
-      <c r="S37" s="202"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
       <c r="T37" s="50"/>
       <c r="U37" s="50"/>
-      <c r="V37" s="202"/>
-      <c r="W37" s="201"/>
-      <c r="X37" s="201"/>
-      <c r="Y37" s="201"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="140"/>
+      <c r="X37" s="140"/>
+      <c r="Y37" s="140"/>
       <c r="Z37" s="50"/>
       <c r="AA37" s="50"/>
       <c r="AB37" s="50"/>
@@ -6103,20 +6100,20 @@
       <c r="I38" s="50"/>
       <c r="J38" s="50"/>
       <c r="K38" s="50"/>
-      <c r="L38" s="202"/>
+      <c r="L38" s="50"/>
       <c r="M38" s="50"/>
       <c r="N38" s="50"/>
-      <c r="O38" s="202"/>
-      <c r="P38" s="202"/>
-      <c r="Q38" s="202"/>
-      <c r="R38" s="202"/>
-      <c r="S38" s="202"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
       <c r="T38" s="50"/>
       <c r="U38" s="50"/>
-      <c r="V38" s="202"/>
-      <c r="W38" s="201"/>
-      <c r="X38" s="201"/>
-      <c r="Y38" s="201"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="140"/>
+      <c r="X38" s="140"/>
+      <c r="Y38" s="140"/>
       <c r="Z38" s="50"/>
       <c r="AA38" s="50"/>
       <c r="AB38" s="50"/>
@@ -6141,20 +6138,20 @@
       <c r="I39" s="50"/>
       <c r="J39" s="50"/>
       <c r="K39" s="50"/>
-      <c r="L39" s="202"/>
+      <c r="L39" s="50"/>
       <c r="M39" s="50"/>
       <c r="N39" s="50"/>
-      <c r="O39" s="202"/>
-      <c r="P39" s="202"/>
-      <c r="Q39" s="202"/>
-      <c r="R39" s="202"/>
-      <c r="S39" s="202"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
       <c r="T39" s="50"/>
       <c r="U39" s="50"/>
-      <c r="V39" s="202"/>
-      <c r="W39" s="201"/>
-      <c r="X39" s="201"/>
-      <c r="Y39" s="201"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="140"/>
+      <c r="X39" s="140"/>
+      <c r="Y39" s="140"/>
       <c r="Z39" s="50"/>
       <c r="AA39" s="50"/>
       <c r="AB39" s="50"/>
@@ -6179,20 +6176,20 @@
       <c r="I40" s="50"/>
       <c r="J40" s="50"/>
       <c r="K40" s="50"/>
-      <c r="L40" s="202"/>
+      <c r="L40" s="50"/>
       <c r="M40" s="50"/>
       <c r="N40" s="50"/>
-      <c r="O40" s="202"/>
-      <c r="P40" s="202"/>
-      <c r="Q40" s="202"/>
-      <c r="R40" s="202"/>
-      <c r="S40" s="202"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
+      <c r="S40" s="50"/>
       <c r="T40" s="50"/>
       <c r="U40" s="50"/>
-      <c r="V40" s="202"/>
-      <c r="W40" s="201"/>
-      <c r="X40" s="201"/>
-      <c r="Y40" s="201"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="140"/>
+      <c r="X40" s="140"/>
+      <c r="Y40" s="140"/>
       <c r="Z40" s="50"/>
       <c r="AA40" s="50"/>
       <c r="AB40" s="50"/>
@@ -6217,20 +6214,20 @@
       <c r="I41" s="50"/>
       <c r="J41" s="50"/>
       <c r="K41" s="50"/>
-      <c r="L41" s="202"/>
+      <c r="L41" s="50"/>
       <c r="M41" s="50"/>
       <c r="N41" s="50"/>
-      <c r="O41" s="202"/>
-      <c r="P41" s="202"/>
-      <c r="Q41" s="202"/>
-      <c r="R41" s="202"/>
-      <c r="S41" s="202"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+      <c r="S41" s="50"/>
       <c r="T41" s="50"/>
       <c r="U41" s="50"/>
-      <c r="V41" s="202"/>
-      <c r="W41" s="201"/>
-      <c r="X41" s="201"/>
-      <c r="Y41" s="201"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="140"/>
+      <c r="X41" s="140"/>
+      <c r="Y41" s="140"/>
       <c r="Z41" s="50"/>
       <c r="AA41" s="50"/>
       <c r="AB41" s="50"/>
@@ -6255,20 +6252,20 @@
       <c r="I42" s="50"/>
       <c r="J42" s="50"/>
       <c r="K42" s="50"/>
-      <c r="L42" s="202"/>
+      <c r="L42" s="50"/>
       <c r="M42" s="50"/>
       <c r="N42" s="50"/>
-      <c r="O42" s="202"/>
-      <c r="P42" s="202"/>
-      <c r="Q42" s="202"/>
-      <c r="R42" s="202"/>
-      <c r="S42" s="202"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50"/>
+      <c r="R42" s="50"/>
+      <c r="S42" s="50"/>
       <c r="T42" s="50"/>
       <c r="U42" s="50"/>
-      <c r="V42" s="202"/>
-      <c r="W42" s="201"/>
-      <c r="X42" s="201"/>
-      <c r="Y42" s="201"/>
+      <c r="V42" s="50"/>
+      <c r="W42" s="140"/>
+      <c r="X42" s="140"/>
+      <c r="Y42" s="140"/>
       <c r="Z42" s="50"/>
       <c r="AA42" s="50"/>
       <c r="AB42" s="50"/>
@@ -6293,20 +6290,20 @@
       <c r="I43" s="50"/>
       <c r="J43" s="50"/>
       <c r="K43" s="50"/>
-      <c r="L43" s="202"/>
+      <c r="L43" s="50"/>
       <c r="M43" s="50"/>
       <c r="N43" s="50"/>
-      <c r="O43" s="202"/>
-      <c r="P43" s="202"/>
-      <c r="Q43" s="202"/>
-      <c r="R43" s="202"/>
-      <c r="S43" s="202"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="50"/>
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
+      <c r="S43" s="50"/>
       <c r="T43" s="50"/>
       <c r="U43" s="50"/>
-      <c r="V43" s="202"/>
-      <c r="W43" s="201"/>
-      <c r="X43" s="201"/>
-      <c r="Y43" s="201"/>
+      <c r="V43" s="50"/>
+      <c r="W43" s="140"/>
+      <c r="X43" s="140"/>
+      <c r="Y43" s="140"/>
       <c r="Z43" s="50"/>
       <c r="AA43" s="50"/>
       <c r="AB43" s="50"/>
@@ -6331,20 +6328,20 @@
       <c r="I44" s="50"/>
       <c r="J44" s="50"/>
       <c r="K44" s="50"/>
-      <c r="L44" s="202"/>
+      <c r="L44" s="50"/>
       <c r="M44" s="50"/>
       <c r="N44" s="50"/>
-      <c r="O44" s="202"/>
-      <c r="P44" s="202"/>
-      <c r="Q44" s="202"/>
-      <c r="R44" s="202"/>
-      <c r="S44" s="202"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
       <c r="T44" s="50"/>
       <c r="U44" s="50"/>
-      <c r="V44" s="202"/>
-      <c r="W44" s="201"/>
-      <c r="X44" s="201"/>
-      <c r="Y44" s="201"/>
+      <c r="V44" s="50"/>
+      <c r="W44" s="140"/>
+      <c r="X44" s="140"/>
+      <c r="Y44" s="140"/>
       <c r="Z44" s="50"/>
       <c r="AA44" s="50"/>
       <c r="AB44" s="50"/>
@@ -6369,20 +6366,20 @@
       <c r="I45" s="50"/>
       <c r="J45" s="50"/>
       <c r="K45" s="50"/>
-      <c r="L45" s="202"/>
+      <c r="L45" s="50"/>
       <c r="M45" s="50"/>
       <c r="N45" s="50"/>
-      <c r="O45" s="202"/>
-      <c r="P45" s="202"/>
-      <c r="Q45" s="202"/>
-      <c r="R45" s="202"/>
-      <c r="S45" s="202"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
+      <c r="S45" s="50"/>
       <c r="T45" s="50"/>
       <c r="U45" s="50"/>
-      <c r="V45" s="202"/>
-      <c r="W45" s="201"/>
-      <c r="X45" s="201"/>
-      <c r="Y45" s="201"/>
+      <c r="V45" s="50"/>
+      <c r="W45" s="140"/>
+      <c r="X45" s="140"/>
+      <c r="Y45" s="140"/>
       <c r="Z45" s="50"/>
       <c r="AA45" s="50"/>
       <c r="AB45" s="50"/>
@@ -6407,20 +6404,20 @@
       <c r="I46" s="50"/>
       <c r="J46" s="50"/>
       <c r="K46" s="50"/>
-      <c r="L46" s="202"/>
+      <c r="L46" s="50"/>
       <c r="M46" s="50"/>
       <c r="N46" s="50"/>
-      <c r="O46" s="202"/>
-      <c r="P46" s="202"/>
-      <c r="Q46" s="202"/>
-      <c r="R46" s="202"/>
-      <c r="S46" s="202"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
       <c r="T46" s="50"/>
       <c r="U46" s="50"/>
-      <c r="V46" s="202"/>
-      <c r="W46" s="201"/>
-      <c r="X46" s="201"/>
-      <c r="Y46" s="201"/>
+      <c r="V46" s="50"/>
+      <c r="W46" s="140"/>
+      <c r="X46" s="140"/>
+      <c r="Y46" s="140"/>
       <c r="Z46" s="50"/>
       <c r="AA46" s="50"/>
       <c r="AB46" s="50"/>
@@ -6445,20 +6442,20 @@
       <c r="I47" s="50"/>
       <c r="J47" s="50"/>
       <c r="K47" s="50"/>
-      <c r="L47" s="202"/>
+      <c r="L47" s="50"/>
       <c r="M47" s="50"/>
       <c r="N47" s="50"/>
-      <c r="O47" s="202"/>
-      <c r="P47" s="202"/>
-      <c r="Q47" s="202"/>
-      <c r="R47" s="202"/>
-      <c r="S47" s="202"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="50"/>
+      <c r="S47" s="50"/>
       <c r="T47" s="50"/>
       <c r="U47" s="50"/>
-      <c r="V47" s="202"/>
-      <c r="W47" s="201"/>
-      <c r="X47" s="201"/>
-      <c r="Y47" s="201"/>
+      <c r="V47" s="50"/>
+      <c r="W47" s="140"/>
+      <c r="X47" s="140"/>
+      <c r="Y47" s="140"/>
       <c r="Z47" s="50"/>
       <c r="AA47" s="50"/>
       <c r="AB47" s="50"/>
@@ -6483,20 +6480,20 @@
       <c r="I48" s="50"/>
       <c r="J48" s="50"/>
       <c r="K48" s="50"/>
-      <c r="L48" s="202"/>
+      <c r="L48" s="50"/>
       <c r="M48" s="50"/>
       <c r="N48" s="50"/>
-      <c r="O48" s="202"/>
-      <c r="P48" s="202"/>
-      <c r="Q48" s="202"/>
-      <c r="R48" s="202"/>
-      <c r="S48" s="202"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="50"/>
+      <c r="S48" s="50"/>
       <c r="T48" s="50"/>
       <c r="U48" s="50"/>
-      <c r="V48" s="202"/>
-      <c r="W48" s="201"/>
-      <c r="X48" s="201"/>
-      <c r="Y48" s="201"/>
+      <c r="V48" s="50"/>
+      <c r="W48" s="140"/>
+      <c r="X48" s="140"/>
+      <c r="Y48" s="140"/>
       <c r="Z48" s="50"/>
       <c r="AA48" s="50"/>
       <c r="AB48" s="50"/>
@@ -6521,20 +6518,20 @@
       <c r="I49" s="50"/>
       <c r="J49" s="50"/>
       <c r="K49" s="50"/>
-      <c r="L49" s="202"/>
+      <c r="L49" s="50"/>
       <c r="M49" s="50"/>
       <c r="N49" s="50"/>
-      <c r="O49" s="202"/>
-      <c r="P49" s="202"/>
-      <c r="Q49" s="202"/>
-      <c r="R49" s="202"/>
-      <c r="S49" s="202"/>
+      <c r="O49" s="50"/>
+      <c r="P49" s="50"/>
+      <c r="Q49" s="50"/>
+      <c r="R49" s="50"/>
+      <c r="S49" s="50"/>
       <c r="T49" s="50"/>
       <c r="U49" s="50"/>
-      <c r="V49" s="202"/>
-      <c r="W49" s="201"/>
-      <c r="X49" s="201"/>
-      <c r="Y49" s="201"/>
+      <c r="V49" s="50"/>
+      <c r="W49" s="140"/>
+      <c r="X49" s="140"/>
+      <c r="Y49" s="140"/>
       <c r="Z49" s="50"/>
       <c r="AA49" s="50"/>
       <c r="AB49" s="50"/>
@@ -6559,20 +6556,20 @@
       <c r="I50" s="50"/>
       <c r="J50" s="50"/>
       <c r="K50" s="50"/>
-      <c r="L50" s="202"/>
+      <c r="L50" s="50"/>
       <c r="M50" s="50"/>
       <c r="N50" s="50"/>
-      <c r="O50" s="202"/>
-      <c r="P50" s="202"/>
-      <c r="Q50" s="202"/>
-      <c r="R50" s="202"/>
-      <c r="S50" s="202"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="50"/>
+      <c r="S50" s="50"/>
       <c r="T50" s="50"/>
       <c r="U50" s="50"/>
-      <c r="V50" s="202"/>
-      <c r="W50" s="201"/>
-      <c r="X50" s="201"/>
-      <c r="Y50" s="201"/>
+      <c r="V50" s="50"/>
+      <c r="W50" s="140"/>
+      <c r="X50" s="140"/>
+      <c r="Y50" s="140"/>
       <c r="Z50" s="50"/>
       <c r="AA50" s="50"/>
       <c r="AB50" s="50"/>
@@ -6597,20 +6594,20 @@
       <c r="I51" s="50"/>
       <c r="J51" s="50"/>
       <c r="K51" s="50"/>
-      <c r="L51" s="202"/>
+      <c r="L51" s="50"/>
       <c r="M51" s="50"/>
       <c r="N51" s="50"/>
-      <c r="O51" s="202"/>
-      <c r="P51" s="202"/>
-      <c r="Q51" s="202"/>
-      <c r="R51" s="202"/>
-      <c r="S51" s="202"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
+      <c r="S51" s="50"/>
       <c r="T51" s="50"/>
       <c r="U51" s="50"/>
-      <c r="V51" s="202"/>
-      <c r="W51" s="201"/>
-      <c r="X51" s="201"/>
-      <c r="Y51" s="201"/>
+      <c r="V51" s="50"/>
+      <c r="W51" s="140"/>
+      <c r="X51" s="140"/>
+      <c r="Y51" s="140"/>
       <c r="Z51" s="50"/>
       <c r="AA51" s="50"/>
       <c r="AB51" s="50"/>
@@ -6635,20 +6632,20 @@
       <c r="I52" s="50"/>
       <c r="J52" s="50"/>
       <c r="K52" s="50"/>
-      <c r="L52" s="202"/>
+      <c r="L52" s="50"/>
       <c r="M52" s="50"/>
       <c r="N52" s="50"/>
-      <c r="O52" s="202"/>
-      <c r="P52" s="202"/>
-      <c r="Q52" s="202"/>
-      <c r="R52" s="202"/>
-      <c r="S52" s="202"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
+      <c r="S52" s="50"/>
       <c r="T52" s="50"/>
       <c r="U52" s="50"/>
-      <c r="V52" s="202"/>
-      <c r="W52" s="201"/>
-      <c r="X52" s="201"/>
-      <c r="Y52" s="201"/>
+      <c r="V52" s="50"/>
+      <c r="W52" s="140"/>
+      <c r="X52" s="140"/>
+      <c r="Y52" s="140"/>
       <c r="Z52" s="50"/>
       <c r="AA52" s="50"/>
       <c r="AB52" s="50"/>
@@ -6673,20 +6670,20 @@
       <c r="I53" s="50"/>
       <c r="J53" s="50"/>
       <c r="K53" s="50"/>
-      <c r="L53" s="202"/>
+      <c r="L53" s="50"/>
       <c r="M53" s="50"/>
       <c r="N53" s="50"/>
-      <c r="O53" s="202"/>
-      <c r="P53" s="202"/>
-      <c r="Q53" s="202"/>
-      <c r="R53" s="202"/>
-      <c r="S53" s="202"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
+      <c r="S53" s="50"/>
       <c r="T53" s="50"/>
       <c r="U53" s="50"/>
-      <c r="V53" s="202"/>
-      <c r="W53" s="201"/>
-      <c r="X53" s="201"/>
-      <c r="Y53" s="201"/>
+      <c r="V53" s="50"/>
+      <c r="W53" s="140"/>
+      <c r="X53" s="140"/>
+      <c r="Y53" s="140"/>
       <c r="Z53" s="50"/>
       <c r="AA53" s="50"/>
       <c r="AB53" s="50"/>
@@ -6711,20 +6708,20 @@
       <c r="I54" s="50"/>
       <c r="J54" s="50"/>
       <c r="K54" s="50"/>
-      <c r="L54" s="202"/>
+      <c r="L54" s="50"/>
       <c r="M54" s="50"/>
       <c r="N54" s="50"/>
-      <c r="O54" s="202"/>
-      <c r="P54" s="202"/>
-      <c r="Q54" s="202"/>
-      <c r="R54" s="202"/>
-      <c r="S54" s="202"/>
+      <c r="O54" s="50"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50"/>
       <c r="T54" s="50"/>
       <c r="U54" s="50"/>
-      <c r="V54" s="202"/>
-      <c r="W54" s="201"/>
-      <c r="X54" s="201"/>
-      <c r="Y54" s="201"/>
+      <c r="V54" s="50"/>
+      <c r="W54" s="140"/>
+      <c r="X54" s="140"/>
+      <c r="Y54" s="140"/>
       <c r="Z54" s="50"/>
       <c r="AA54" s="50"/>
       <c r="AB54" s="50"/>
@@ -6749,20 +6746,20 @@
       <c r="I55" s="50"/>
       <c r="J55" s="50"/>
       <c r="K55" s="50"/>
-      <c r="L55" s="202"/>
+      <c r="L55" s="50"/>
       <c r="M55" s="50"/>
       <c r="N55" s="50"/>
-      <c r="O55" s="202"/>
-      <c r="P55" s="202"/>
-      <c r="Q55" s="202"/>
-      <c r="R55" s="202"/>
-      <c r="S55" s="202"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50"/>
       <c r="T55" s="50"/>
       <c r="U55" s="50"/>
-      <c r="V55" s="202"/>
-      <c r="W55" s="201"/>
-      <c r="X55" s="201"/>
-      <c r="Y55" s="201"/>
+      <c r="V55" s="50"/>
+      <c r="W55" s="140"/>
+      <c r="X55" s="140"/>
+      <c r="Y55" s="140"/>
       <c r="Z55" s="50"/>
       <c r="AA55" s="50"/>
       <c r="AB55" s="50"/>
@@ -6787,20 +6784,20 @@
       <c r="I56" s="50"/>
       <c r="J56" s="50"/>
       <c r="K56" s="50"/>
-      <c r="L56" s="202"/>
+      <c r="L56" s="50"/>
       <c r="M56" s="50"/>
       <c r="N56" s="50"/>
-      <c r="O56" s="202"/>
-      <c r="P56" s="202"/>
-      <c r="Q56" s="202"/>
-      <c r="R56" s="202"/>
-      <c r="S56" s="202"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="50"/>
       <c r="T56" s="50"/>
       <c r="U56" s="50"/>
-      <c r="V56" s="202"/>
-      <c r="W56" s="201"/>
-      <c r="X56" s="201"/>
-      <c r="Y56" s="201"/>
+      <c r="V56" s="50"/>
+      <c r="W56" s="140"/>
+      <c r="X56" s="140"/>
+      <c r="Y56" s="140"/>
       <c r="Z56" s="50"/>
       <c r="AA56" s="50"/>
       <c r="AB56" s="50"/>
@@ -6814,7 +6811,7 @@
       <c r="AJ56" s="73"/>
     </row>
     <row r="57" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A57" s="200"/>
+      <c r="A57" s="139"/>
       <c r="B57" s="89"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
@@ -6825,20 +6822,20 @@
       <c r="I57" s="50"/>
       <c r="J57" s="50"/>
       <c r="K57" s="50"/>
-      <c r="L57" s="202"/>
+      <c r="L57" s="50"/>
       <c r="M57" s="50"/>
       <c r="N57" s="50"/>
-      <c r="O57" s="202"/>
-      <c r="P57" s="202"/>
-      <c r="Q57" s="202"/>
-      <c r="R57" s="202"/>
-      <c r="S57" s="202"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="50"/>
+      <c r="S57" s="50"/>
       <c r="T57" s="50"/>
       <c r="U57" s="50"/>
-      <c r="V57" s="202"/>
-      <c r="W57" s="201"/>
-      <c r="X57" s="201"/>
-      <c r="Y57" s="201"/>
+      <c r="V57" s="50"/>
+      <c r="W57" s="140"/>
+      <c r="X57" s="140"/>
+      <c r="Y57" s="140"/>
       <c r="Z57" s="50"/>
       <c r="AA57" s="50"/>
       <c r="AB57" s="50"/>
@@ -6866,20 +6863,20 @@
       <c r="I58" s="50"/>
       <c r="J58" s="50"/>
       <c r="K58" s="50"/>
-      <c r="L58" s="202"/>
+      <c r="L58" s="50"/>
       <c r="M58" s="50"/>
       <c r="N58" s="50"/>
-      <c r="O58" s="202"/>
-      <c r="P58" s="202"/>
-      <c r="Q58" s="202"/>
-      <c r="R58" s="202"/>
-      <c r="S58" s="202"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="50"/>
+      <c r="Q58" s="50"/>
+      <c r="R58" s="50"/>
+      <c r="S58" s="50"/>
       <c r="T58" s="50"/>
       <c r="U58" s="50"/>
-      <c r="V58" s="202"/>
-      <c r="W58" s="201"/>
-      <c r="X58" s="201"/>
-      <c r="Y58" s="201"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="140"/>
+      <c r="X58" s="140"/>
+      <c r="Y58" s="140"/>
       <c r="Z58" s="50"/>
       <c r="AA58" s="50"/>
       <c r="AB58" s="50"/>
@@ -6907,20 +6904,20 @@
       <c r="I59" s="50"/>
       <c r="J59" s="50"/>
       <c r="K59" s="50"/>
-      <c r="L59" s="202"/>
+      <c r="L59" s="50"/>
       <c r="M59" s="50"/>
       <c r="N59" s="50"/>
-      <c r="O59" s="202"/>
-      <c r="P59" s="202"/>
-      <c r="Q59" s="202"/>
-      <c r="R59" s="202"/>
-      <c r="S59" s="202"/>
+      <c r="O59" s="50"/>
+      <c r="P59" s="50"/>
+      <c r="Q59" s="50"/>
+      <c r="R59" s="50"/>
+      <c r="S59" s="50"/>
       <c r="T59" s="50"/>
       <c r="U59" s="50"/>
-      <c r="V59" s="202"/>
-      <c r="W59" s="201"/>
-      <c r="X59" s="201"/>
-      <c r="Y59" s="201"/>
+      <c r="V59" s="50"/>
+      <c r="W59" s="140"/>
+      <c r="X59" s="140"/>
+      <c r="Y59" s="140"/>
       <c r="Z59" s="50"/>
       <c r="AA59" s="50"/>
       <c r="AB59" s="50"/>
@@ -6948,20 +6945,20 @@
       <c r="I60" s="50"/>
       <c r="J60" s="50"/>
       <c r="K60" s="50"/>
-      <c r="L60" s="202"/>
+      <c r="L60" s="50"/>
       <c r="M60" s="50"/>
       <c r="N60" s="50"/>
-      <c r="O60" s="202"/>
-      <c r="P60" s="202"/>
-      <c r="Q60" s="202"/>
-      <c r="R60" s="202"/>
-      <c r="S60" s="202"/>
+      <c r="O60" s="50"/>
+      <c r="P60" s="50"/>
+      <c r="Q60" s="50"/>
+      <c r="R60" s="50"/>
+      <c r="S60" s="50"/>
       <c r="T60" s="50"/>
       <c r="U60" s="50"/>
-      <c r="V60" s="202"/>
-      <c r="W60" s="201"/>
-      <c r="X60" s="201"/>
-      <c r="Y60" s="201"/>
+      <c r="V60" s="50"/>
+      <c r="W60" s="140"/>
+      <c r="X60" s="140"/>
+      <c r="Y60" s="140"/>
       <c r="Z60" s="50"/>
       <c r="AA60" s="50"/>
       <c r="AB60" s="50"/>
@@ -7211,11 +7208,11 @@
       <c r="AJ65" s="73"/>
     </row>
     <row r="66" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A66" s="176" t="s">
+      <c r="A66" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="177"/>
-      <c r="C66" s="178"/>
+      <c r="B66" s="146"/>
+      <c r="C66" s="147"/>
       <c r="D66" s="57"/>
       <c r="E66" s="57"/>
       <c r="F66" s="57"/>
@@ -7260,11 +7257,11 @@
       <c r="AJ66" s="73"/>
     </row>
     <row r="67" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A67" s="176" t="s">
+      <c r="A67" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="177"/>
-      <c r="C67" s="178"/>
+      <c r="B67" s="146"/>
+      <c r="C67" s="147"/>
       <c r="D67" s="57"/>
       <c r="E67" s="57"/>
       <c r="F67" s="57"/>
@@ -7303,11 +7300,11 @@
       <c r="AJ67" s="73"/>
     </row>
     <row r="68" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A68" s="179" t="s">
+      <c r="A68" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="B68" s="180"/>
-      <c r="C68" s="181"/>
+      <c r="B68" s="149"/>
+      <c r="C68" s="150"/>
       <c r="D68" s="57"/>
       <c r="E68" s="57"/>
       <c r="F68" s="57"/>
@@ -7360,11 +7357,11 @@
       <c r="AJ68" s="73"/>
     </row>
     <row r="69" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A69" s="176" t="s">
+      <c r="A69" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="B69" s="177"/>
-      <c r="C69" s="178"/>
+      <c r="B69" s="146"/>
+      <c r="C69" s="147"/>
       <c r="D69" s="57">
         <f t="shared" ref="D69:AC69" si="3">SUM(D11:D64)</f>
         <v>1</v>
@@ -7502,145 +7499,145 @@
         <v>42</v>
       </c>
       <c r="D71" s="4"/>
-      <c r="E71" s="143"/>
-      <c r="F71" s="143"/>
-      <c r="G71" s="143"/>
-      <c r="H71" s="143"/>
-      <c r="I71" s="143"/>
-      <c r="J71" s="143"/>
-      <c r="S71" s="196" t="s">
+      <c r="E71" s="154"/>
+      <c r="F71" s="154"/>
+      <c r="G71" s="154"/>
+      <c r="H71" s="154"/>
+      <c r="I71" s="154"/>
+      <c r="J71" s="154"/>
+      <c r="S71" s="199" t="s">
         <v>43</v>
       </c>
-      <c r="T71" s="197"/>
-      <c r="U71" s="197"/>
-      <c r="V71" s="197"/>
-      <c r="W71" s="197"/>
-      <c r="X71" s="197"/>
-      <c r="Y71" s="197"/>
-      <c r="Z71" s="197"/>
-      <c r="AA71" s="198"/>
-      <c r="AC71" s="182" t="s">
+      <c r="T71" s="200"/>
+      <c r="U71" s="200"/>
+      <c r="V71" s="200"/>
+      <c r="W71" s="200"/>
+      <c r="X71" s="200"/>
+      <c r="Y71" s="200"/>
+      <c r="Z71" s="200"/>
+      <c r="AA71" s="201"/>
+      <c r="AC71" s="185" t="s">
         <v>173</v>
       </c>
-      <c r="AD71" s="183"/>
-      <c r="AE71" s="183"/>
-      <c r="AF71" s="183"/>
-      <c r="AG71" s="183"/>
-      <c r="AH71" s="183"/>
-      <c r="AI71" s="183"/>
-      <c r="AJ71" s="184"/>
+      <c r="AD71" s="186"/>
+      <c r="AE71" s="186"/>
+      <c r="AF71" s="186"/>
+      <c r="AG71" s="186"/>
+      <c r="AH71" s="186"/>
+      <c r="AI71" s="186"/>
+      <c r="AJ71" s="187"/>
     </row>
     <row r="72" spans="1:36" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="69"/>
       <c r="B72" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E72" s="143"/>
-      <c r="F72" s="143"/>
-      <c r="G72" s="143"/>
-      <c r="H72" s="143"/>
-      <c r="I72" s="143"/>
-      <c r="J72" s="143"/>
-      <c r="S72" s="185" t="s">
+      <c r="E72" s="154"/>
+      <c r="F72" s="154"/>
+      <c r="G72" s="154"/>
+      <c r="H72" s="154"/>
+      <c r="I72" s="154"/>
+      <c r="J72" s="154"/>
+      <c r="S72" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="T72" s="186"/>
-      <c r="U72" s="187" t="s">
+      <c r="T72" s="189"/>
+      <c r="U72" s="190" t="s">
         <v>170</v>
       </c>
-      <c r="V72" s="187"/>
-      <c r="W72" s="187"/>
-      <c r="X72" s="187"/>
-      <c r="Y72" s="187"/>
-      <c r="Z72" s="187"/>
-      <c r="AA72" s="188"/>
-      <c r="AC72" s="159" t="s">
+      <c r="V72" s="190"/>
+      <c r="W72" s="190"/>
+      <c r="X72" s="190"/>
+      <c r="Y72" s="190"/>
+      <c r="Z72" s="190"/>
+      <c r="AA72" s="191"/>
+      <c r="AC72" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="AD72" s="145"/>
-      <c r="AE72" s="145"/>
-      <c r="AF72" s="145"/>
-      <c r="AG72" s="145"/>
-      <c r="AH72" s="145"/>
-      <c r="AI72" s="145"/>
-      <c r="AJ72" s="146"/>
+      <c r="AD72" s="156"/>
+      <c r="AE72" s="156"/>
+      <c r="AF72" s="156"/>
+      <c r="AG72" s="156"/>
+      <c r="AH72" s="156"/>
+      <c r="AI72" s="156"/>
+      <c r="AJ72" s="157"/>
     </row>
     <row r="73" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="70"/>
       <c r="B73" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E73" s="143"/>
-      <c r="F73" s="143"/>
-      <c r="G73" s="143"/>
-      <c r="H73" s="143"/>
-      <c r="I73" s="143"/>
-      <c r="J73" s="143"/>
-      <c r="S73" s="185"/>
-      <c r="T73" s="186"/>
-      <c r="U73" s="187"/>
-      <c r="V73" s="187"/>
-      <c r="W73" s="187"/>
-      <c r="X73" s="187"/>
-      <c r="Y73" s="187"/>
-      <c r="Z73" s="187"/>
-      <c r="AA73" s="188"/>
-      <c r="AC73" s="160"/>
-      <c r="AD73" s="148"/>
-      <c r="AE73" s="148"/>
-      <c r="AF73" s="148"/>
-      <c r="AG73" s="148"/>
-      <c r="AH73" s="148"/>
-      <c r="AI73" s="148"/>
-      <c r="AJ73" s="149"/>
+      <c r="E73" s="154"/>
+      <c r="F73" s="154"/>
+      <c r="G73" s="154"/>
+      <c r="H73" s="154"/>
+      <c r="I73" s="154"/>
+      <c r="J73" s="154"/>
+      <c r="S73" s="188"/>
+      <c r="T73" s="189"/>
+      <c r="U73" s="190"/>
+      <c r="V73" s="190"/>
+      <c r="W73" s="190"/>
+      <c r="X73" s="190"/>
+      <c r="Y73" s="190"/>
+      <c r="Z73" s="190"/>
+      <c r="AA73" s="191"/>
+      <c r="AC73" s="171"/>
+      <c r="AD73" s="159"/>
+      <c r="AE73" s="159"/>
+      <c r="AF73" s="159"/>
+      <c r="AG73" s="159"/>
+      <c r="AH73" s="159"/>
+      <c r="AI73" s="159"/>
+      <c r="AJ73" s="160"/>
     </row>
     <row r="74" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="71"/>
       <c r="B74" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E74" s="143"/>
-      <c r="F74" s="143"/>
-      <c r="G74" s="143"/>
-      <c r="H74" s="143"/>
-      <c r="I74" s="143"/>
-      <c r="J74" s="143"/>
-      <c r="S74" s="185"/>
-      <c r="T74" s="186"/>
-      <c r="U74" s="187"/>
-      <c r="V74" s="187"/>
-      <c r="W74" s="187"/>
-      <c r="X74" s="187"/>
-      <c r="Y74" s="187"/>
-      <c r="Z74" s="187"/>
-      <c r="AA74" s="188"/>
-      <c r="AC74" s="160"/>
-      <c r="AD74" s="148"/>
-      <c r="AE74" s="148"/>
-      <c r="AF74" s="148"/>
-      <c r="AG74" s="148"/>
-      <c r="AH74" s="148"/>
-      <c r="AI74" s="148"/>
-      <c r="AJ74" s="149"/>
+      <c r="E74" s="154"/>
+      <c r="F74" s="154"/>
+      <c r="G74" s="154"/>
+      <c r="H74" s="154"/>
+      <c r="I74" s="154"/>
+      <c r="J74" s="154"/>
+      <c r="S74" s="188"/>
+      <c r="T74" s="189"/>
+      <c r="U74" s="190"/>
+      <c r="V74" s="190"/>
+      <c r="W74" s="190"/>
+      <c r="X74" s="190"/>
+      <c r="Y74" s="190"/>
+      <c r="Z74" s="190"/>
+      <c r="AA74" s="191"/>
+      <c r="AC74" s="171"/>
+      <c r="AD74" s="159"/>
+      <c r="AE74" s="159"/>
+      <c r="AF74" s="159"/>
+      <c r="AG74" s="159"/>
+      <c r="AH74" s="159"/>
+      <c r="AI74" s="159"/>
+      <c r="AJ74" s="160"/>
     </row>
     <row r="75" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S75" s="185"/>
-      <c r="T75" s="186"/>
-      <c r="U75" s="187"/>
-      <c r="V75" s="187"/>
-      <c r="W75" s="187"/>
-      <c r="X75" s="187"/>
-      <c r="Y75" s="187"/>
-      <c r="Z75" s="187"/>
-      <c r="AA75" s="188"/>
-      <c r="AC75" s="160"/>
-      <c r="AD75" s="148"/>
-      <c r="AE75" s="148"/>
-      <c r="AF75" s="148"/>
-      <c r="AG75" s="148"/>
-      <c r="AH75" s="148"/>
-      <c r="AI75" s="148"/>
-      <c r="AJ75" s="149"/>
+      <c r="S75" s="188"/>
+      <c r="T75" s="189"/>
+      <c r="U75" s="190"/>
+      <c r="V75" s="190"/>
+      <c r="W75" s="190"/>
+      <c r="X75" s="190"/>
+      <c r="Y75" s="190"/>
+      <c r="Z75" s="190"/>
+      <c r="AA75" s="191"/>
+      <c r="AC75" s="171"/>
+      <c r="AD75" s="159"/>
+      <c r="AE75" s="159"/>
+      <c r="AF75" s="159"/>
+      <c r="AG75" s="159"/>
+      <c r="AH75" s="159"/>
+      <c r="AI75" s="159"/>
+      <c r="AJ75" s="160"/>
     </row>
     <row r="76" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A76" s="72" t="s">
@@ -7653,29 +7650,29 @@
       <c r="F76" s="44"/>
       <c r="G76" s="44"/>
       <c r="H76" s="44"/>
-      <c r="S76" s="185"/>
-      <c r="T76" s="186"/>
-      <c r="U76" s="187"/>
-      <c r="V76" s="187"/>
-      <c r="W76" s="187"/>
-      <c r="X76" s="187"/>
-      <c r="Y76" s="187"/>
-      <c r="Z76" s="187"/>
-      <c r="AA76" s="188"/>
-      <c r="AC76" s="189"/>
-      <c r="AD76" s="190"/>
-      <c r="AE76" s="190"/>
-      <c r="AF76" s="190"/>
-      <c r="AG76" s="190"/>
-      <c r="AH76" s="190"/>
-      <c r="AI76" s="190"/>
-      <c r="AJ76" s="191"/>
+      <c r="S76" s="188"/>
+      <c r="T76" s="189"/>
+      <c r="U76" s="190"/>
+      <c r="V76" s="190"/>
+      <c r="W76" s="190"/>
+      <c r="X76" s="190"/>
+      <c r="Y76" s="190"/>
+      <c r="Z76" s="190"/>
+      <c r="AA76" s="191"/>
+      <c r="AC76" s="192"/>
+      <c r="AD76" s="193"/>
+      <c r="AE76" s="193"/>
+      <c r="AF76" s="193"/>
+      <c r="AG76" s="193"/>
+      <c r="AH76" s="193"/>
+      <c r="AI76" s="193"/>
+      <c r="AJ76" s="194"/>
     </row>
     <row r="77" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A77" s="140" t="s">
+      <c r="A77" s="151" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="140"/>
+      <c r="B77" s="151"/>
       <c r="C77" s="63">
         <f>COUNTIF(D68:AH68,"=8")</f>
         <v>7</v>
@@ -7685,29 +7682,29 @@
       <c r="F77" s="44"/>
       <c r="G77" s="44"/>
       <c r="H77" s="44"/>
-      <c r="S77" s="185" t="s">
+      <c r="S77" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="T77" s="186"/>
-      <c r="U77" s="187" t="s">
+      <c r="T77" s="189"/>
+      <c r="U77" s="190" t="s">
         <v>171</v>
       </c>
-      <c r="V77" s="187"/>
-      <c r="W77" s="187"/>
-      <c r="X77" s="187"/>
-      <c r="Y77" s="187"/>
-      <c r="Z77" s="187"/>
-      <c r="AA77" s="188"/>
-      <c r="AC77" s="160" t="s">
+      <c r="V77" s="190"/>
+      <c r="W77" s="190"/>
+      <c r="X77" s="190"/>
+      <c r="Y77" s="190"/>
+      <c r="Z77" s="190"/>
+      <c r="AA77" s="191"/>
+      <c r="AC77" s="171" t="s">
         <v>172</v>
       </c>
-      <c r="AD77" s="148"/>
-      <c r="AE77" s="148"/>
-      <c r="AF77" s="148"/>
-      <c r="AG77" s="148"/>
-      <c r="AH77" s="148"/>
-      <c r="AI77" s="148"/>
-      <c r="AJ77" s="149"/>
+      <c r="AD77" s="159"/>
+      <c r="AE77" s="159"/>
+      <c r="AF77" s="159"/>
+      <c r="AG77" s="159"/>
+      <c r="AH77" s="159"/>
+      <c r="AI77" s="159"/>
+      <c r="AJ77" s="160"/>
     </row>
     <row r="78" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A78" s="63" t="s">
@@ -7723,23 +7720,23 @@
       <c r="F78" s="44"/>
       <c r="G78" s="44"/>
       <c r="H78" s="44"/>
-      <c r="S78" s="185"/>
-      <c r="T78" s="186"/>
-      <c r="U78" s="187"/>
-      <c r="V78" s="187"/>
-      <c r="W78" s="187"/>
-      <c r="X78" s="187"/>
-      <c r="Y78" s="187"/>
-      <c r="Z78" s="187"/>
-      <c r="AA78" s="188"/>
-      <c r="AC78" s="160"/>
-      <c r="AD78" s="148"/>
-      <c r="AE78" s="148"/>
-      <c r="AF78" s="148"/>
-      <c r="AG78" s="148"/>
-      <c r="AH78" s="148"/>
-      <c r="AI78" s="148"/>
-      <c r="AJ78" s="149"/>
+      <c r="S78" s="188"/>
+      <c r="T78" s="189"/>
+      <c r="U78" s="190"/>
+      <c r="V78" s="190"/>
+      <c r="W78" s="190"/>
+      <c r="X78" s="190"/>
+      <c r="Y78" s="190"/>
+      <c r="Z78" s="190"/>
+      <c r="AA78" s="191"/>
+      <c r="AC78" s="171"/>
+      <c r="AD78" s="159"/>
+      <c r="AE78" s="159"/>
+      <c r="AF78" s="159"/>
+      <c r="AG78" s="159"/>
+      <c r="AH78" s="159"/>
+      <c r="AI78" s="159"/>
+      <c r="AJ78" s="160"/>
     </row>
     <row r="79" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A79" s="63" t="s">
@@ -7755,23 +7752,23 @@
       <c r="F79" s="44"/>
       <c r="G79" s="44"/>
       <c r="H79" s="44"/>
-      <c r="S79" s="185"/>
-      <c r="T79" s="186"/>
-      <c r="U79" s="187"/>
-      <c r="V79" s="187"/>
-      <c r="W79" s="187"/>
-      <c r="X79" s="187"/>
-      <c r="Y79" s="187"/>
-      <c r="Z79" s="187"/>
-      <c r="AA79" s="188"/>
-      <c r="AC79" s="160"/>
-      <c r="AD79" s="148"/>
-      <c r="AE79" s="148"/>
-      <c r="AF79" s="148"/>
-      <c r="AG79" s="148"/>
-      <c r="AH79" s="148"/>
-      <c r="AI79" s="148"/>
-      <c r="AJ79" s="149"/>
+      <c r="S79" s="188"/>
+      <c r="T79" s="189"/>
+      <c r="U79" s="190"/>
+      <c r="V79" s="190"/>
+      <c r="W79" s="190"/>
+      <c r="X79" s="190"/>
+      <c r="Y79" s="190"/>
+      <c r="Z79" s="190"/>
+      <c r="AA79" s="191"/>
+      <c r="AC79" s="171"/>
+      <c r="AD79" s="159"/>
+      <c r="AE79" s="159"/>
+      <c r="AF79" s="159"/>
+      <c r="AG79" s="159"/>
+      <c r="AH79" s="159"/>
+      <c r="AI79" s="159"/>
+      <c r="AJ79" s="160"/>
     </row>
     <row r="80" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A80" s="63" t="s">
@@ -7787,29 +7784,29 @@
       <c r="F80" s="44"/>
       <c r="G80" s="44"/>
       <c r="H80" s="44"/>
-      <c r="S80" s="185"/>
-      <c r="T80" s="186"/>
-      <c r="U80" s="187"/>
-      <c r="V80" s="187"/>
-      <c r="W80" s="187"/>
-      <c r="X80" s="187"/>
-      <c r="Y80" s="187"/>
-      <c r="Z80" s="187"/>
-      <c r="AA80" s="188"/>
-      <c r="AC80" s="160"/>
-      <c r="AD80" s="148"/>
-      <c r="AE80" s="148"/>
-      <c r="AF80" s="148"/>
-      <c r="AG80" s="148"/>
-      <c r="AH80" s="148"/>
-      <c r="AI80" s="148"/>
-      <c r="AJ80" s="149"/>
+      <c r="S80" s="188"/>
+      <c r="T80" s="189"/>
+      <c r="U80" s="190"/>
+      <c r="V80" s="190"/>
+      <c r="W80" s="190"/>
+      <c r="X80" s="190"/>
+      <c r="Y80" s="190"/>
+      <c r="Z80" s="190"/>
+      <c r="AA80" s="191"/>
+      <c r="AC80" s="171"/>
+      <c r="AD80" s="159"/>
+      <c r="AE80" s="159"/>
+      <c r="AF80" s="159"/>
+      <c r="AG80" s="159"/>
+      <c r="AH80" s="159"/>
+      <c r="AI80" s="159"/>
+      <c r="AJ80" s="160"/>
     </row>
     <row r="81" spans="1:36" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A81" s="174" t="s">
+      <c r="A81" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="B81" s="174"/>
+      <c r="B81" s="142"/>
       <c r="C81" s="63">
         <f>COUNTIF(D69:AH69,"&gt;0")</f>
         <v>12</v>
@@ -7819,23 +7816,23 @@
       <c r="F81" s="44"/>
       <c r="G81" s="44"/>
       <c r="H81" s="44"/>
-      <c r="S81" s="192"/>
-      <c r="T81" s="193"/>
-      <c r="U81" s="194"/>
-      <c r="V81" s="194"/>
-      <c r="W81" s="194"/>
-      <c r="X81" s="194"/>
-      <c r="Y81" s="194"/>
-      <c r="Z81" s="194"/>
-      <c r="AA81" s="195"/>
-      <c r="AC81" s="161"/>
-      <c r="AD81" s="151"/>
-      <c r="AE81" s="151"/>
-      <c r="AF81" s="151"/>
-      <c r="AG81" s="151"/>
-      <c r="AH81" s="151"/>
-      <c r="AI81" s="151"/>
-      <c r="AJ81" s="152"/>
+      <c r="S81" s="195"/>
+      <c r="T81" s="196"/>
+      <c r="U81" s="197"/>
+      <c r="V81" s="197"/>
+      <c r="W81" s="197"/>
+      <c r="X81" s="197"/>
+      <c r="Y81" s="197"/>
+      <c r="Z81" s="197"/>
+      <c r="AA81" s="198"/>
+      <c r="AC81" s="172"/>
+      <c r="AD81" s="162"/>
+      <c r="AE81" s="162"/>
+      <c r="AF81" s="162"/>
+      <c r="AG81" s="162"/>
+      <c r="AH81" s="162"/>
+      <c r="AI81" s="162"/>
+      <c r="AJ81" s="163"/>
     </row>
     <row r="82" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A82" s="63" t="s">
@@ -7875,10 +7872,10 @@
       <c r="H84" s="44"/>
     </row>
     <row r="85" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="174" t="s">
+      <c r="A85" s="142" t="s">
         <v>62</v>
       </c>
-      <c r="B85" s="174"/>
+      <c r="B85" s="142"/>
       <c r="C85" s="63">
         <f>AI69</f>
         <v>12</v>
@@ -7890,10 +7887,10 @@
       <c r="H85" s="44"/>
     </row>
     <row r="86" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="174" t="s">
+      <c r="A86" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="B86" s="174"/>
+      <c r="B86" s="142"/>
       <c r="C86" s="63">
         <v>39</v>
       </c>
@@ -8022,17 +8019,6 @@
     <row r="97" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="AI9:AI10"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="E71:J74"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="AC71:AJ71"/>
@@ -8045,6 +8031,17 @@
     <mergeCell ref="AC77:AJ81"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="S71:AA71"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="E71:J74"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="expression" dxfId="5" priority="1">
@@ -8943,7 +8940,7 @@
       <c r="C47" s="129"/>
       <c r="D47" s="122"/>
       <c r="E47" s="119"/>
-      <c r="F47" s="199"/>
+      <c r="F47" s="202"/>
       <c r="G47" s="122"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.35">
@@ -8951,7 +8948,7 @@
       <c r="C48" s="128"/>
       <c r="D48" s="122"/>
       <c r="E48" s="119"/>
-      <c r="F48" s="199"/>
+      <c r="F48" s="202"/>
       <c r="G48" s="122"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.35">
@@ -8959,7 +8956,7 @@
       <c r="C49" s="128"/>
       <c r="D49" s="122"/>
       <c r="E49" s="119"/>
-      <c r="F49" s="199"/>
+      <c r="F49" s="202"/>
       <c r="G49" s="122"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
@@ -8967,7 +8964,7 @@
       <c r="C50" s="129"/>
       <c r="D50" s="122"/>
       <c r="E50" s="119"/>
-      <c r="F50" s="199"/>
+      <c r="F50" s="202"/>
       <c r="G50" s="122"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">
@@ -9128,15 +9125,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CBBA4E8384962545BF977EF5EB207524" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4c71af4b5276cc520d7caa7153b08011">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ecef1726-c816-4ce0-a2de-c7222e5e0303" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d40dcfb130600d1adddbff1088e0e0d5" ns2:_="">
     <xsd:import namespace="ecef1726-c816-4ce0-a2de-c7222e5e0303"/>
@@ -9280,15 +9268,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A50F55-EB9E-48CA-A399-9CBC9253A5CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1BDC32-896F-448F-9DE0-A2D567D26AC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9304,4 +9293,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A50F55-EB9E-48CA-A399-9CBC9253A5CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>